<commit_message>
feat(apache-poi): add gender validator and clean up unused code
</commit_message>
<xml_diff>
--- a/commons-apache-poi/src/test/resources/sample/sample-1.xlsx
+++ b/commons-apache-poi/src/test/resources/sample/sample-1.xlsx
@@ -27,7 +27,7 @@
         <t>사용자 역할은 'MANAGER', 'USER' 만 가능합니다.</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <t>활성화는 'Y'/'N' 입력만 가능합니다.</t>
       </text>
@@ -84,7 +84,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -113,10 +113,15 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>사용자 성별</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>이메일</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>활성화</t>
         </is>
@@ -125,7 +130,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>userwDqSKYOpR8</t>
+          <t>userR9XAqVHCaD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -135,16 +140,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DvWcNsslgq</t>
+          <t>MnjaAyvTSj</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>USER</t>
+          <t>MANAGER</t>
         </is>
       </c>
-      <c r="E2"/>
-      <c r="F2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>N</t>
         </is>

</xml_diff>